<commit_message>
Added logger information and comments
</commit_message>
<xml_diff>
--- a/testdata/testData.xlsx
+++ b/testdata/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhai.kumar/Documents/ProtractorTest/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manasp/Documents/ProtractorTest/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C2D6A9-29FC-EF40-9892-D831A7D24B25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47D14D4-1C2C-E443-AB3D-DBCDC47F16A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{6EBB8116-2124-7B45-A0CE-187D17D74F7A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" activeTab="1" xr2:uid="{6EBB8116-2124-7B45-A0CE-187D17D74F7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Abhai" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>code</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>output</t>
-  </si>
-  <si>
-    <t>abhai</t>
   </si>
 </sst>
 </file>
@@ -469,10 +466,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAEFBBA-618B-7F44-81C0-30893D9265B2}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,7 +479,7 @@
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -492,11 +489,8 @@
       <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -506,25 +500,19 @@
       <c r="C2">
         <v>30</v>
       </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -532,9 +520,6 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4">
         <v>9</v>
       </c>
     </row>

</xml_diff>